<commit_message>
Capitalize the month of May in report template
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_12_rpt_CF_InvoicePaymentsbyPortfolio.xlsx
+++ b/backend/reports/xlsx/Tab_12_rpt_CF_InvoicePaymentsbyPortfolio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleshapka/Development/github/gdx-agreements-tracker/backend/reports/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anlashle/Repos/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD528B9-C45D-544A-8CC5-4FDBB43108C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E6E54E-204E-3241-B6F3-E3FD60C55025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37620" yWindow="20" windowWidth="34560" windowHeight="19700" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>Apr</t>
   </si>
   <si>
-    <t>may</t>
-  </si>
-  <si>
     <t>Jun</t>
   </si>
   <si>
@@ -300,6 +297,9 @@
   </si>
   <si>
     <t>{$p1.co_number}</t>
+  </si>
+  <si>
+    <t>May</t>
   </si>
 </sst>
 </file>
@@ -517,11 +517,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -541,6 +537,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,9 +620,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -660,7 +660,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -766,7 +766,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -908,7 +908,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -922,7 +922,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -933,31 +933,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" ht="57" customHeight="1">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-    </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+    </row>
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="17" thickBot="1">
       <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
@@ -982,7 +982,7 @@
       <c r="T2" s="14"/>
       <c r="U2" s="14"/>
     </row>
-    <row r="3" spans="1:21" s="1" customFormat="1" ht="20" thickBot="1">
+    <row r="3" spans="1:21" s="1" customFormat="1" ht="17" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1008,113 +1008,113 @@
         <v>12</v>
       </c>
       <c r="I3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="6" t="s">
+    </row>
+    <row r="4" spans="1:21" s="2" customFormat="1" ht="17" thickBot="1">
+      <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="C4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="L4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="Q4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="R4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="S4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="T4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="U4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="U4" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" s="2" customFormat="1" ht="20" thickBot="1">
+    </row>
+    <row r="5" spans="1:21" s="2" customFormat="1" ht="17" thickBot="1">
       <c r="A5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
@@ -1137,168 +1137,168 @@
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
     </row>
-    <row r="6" spans="1:21" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="22" t="s">
+    <row r="6" spans="1:21" s="1" customFormat="1" ht="17" thickBot="1">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="S6" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="T6" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="U6" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="17" thickBot="1">
+      <c r="A7" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="17" thickBot="1">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="K6" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="L6" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="M6" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="N6" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="O6" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="P6" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q6" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="R6" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="S6" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="T6" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="U6" s="21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="17" thickBot="1">
-      <c r="A7" s="18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="17" thickBot="1">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="24" t="s">
+      <c r="F8" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="P8" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q8" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="R8" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="S8" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="T8" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="U8" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="21"/>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="F8" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="J8" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="K8" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="L8" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="M8" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="N8" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="O8" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="P8" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q8" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="R8" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="S8" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="T8" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="U8" s="21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="19">
-      <c r="A9" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="19">
-      <c r="A10" s="23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="19">
-      <c r="A11" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="19">
-      <c r="A12" s="23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="19">
-      <c r="A13" s="23"/>
-    </row>
-    <row r="14" spans="1:21" ht="19">
-      <c r="A14" s="23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="19">
-      <c r="A15" s="23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="19">
-      <c r="A16" s="23"/>
-    </row>
-    <row r="17" spans="1:1" ht="19">
-      <c r="A17" s="23" t="s">
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="21"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="19">
-      <c r="A18" s="23" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" s="21" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>